<commit_message>
Journal de travail edit Simon Cuany
</commit_message>
<xml_diff>
--- a/Journaux de travail/Journal_SimonCuany.xlsx
+++ b/Journaux de travail/Journal_SimonCuany.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\simon.cuany\Documents\GitHub\ProjetWeb_Annonces\Journeaux de travaille\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\simon.cuany\Documents\GitHub\ProjetWeb_Annonces\Journaux de travail\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3960" yWindow="0" windowWidth="28800" windowHeight="12330"/>
+    <workbookView xWindow="4950" yWindow="0" windowWidth="28800" windowHeight="12330"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="35">
   <si>
     <t>Date</t>
   </si>
@@ -108,6 +108,27 @@
   </si>
   <si>
     <t>Modification du style de la page register ainsi que du login et du gabarit. Créer la page de création d'annonces modifier l'index en ajoutant une nouvelle case au switch. Modification du journal de travaille</t>
+  </si>
+  <si>
+    <t>12h15</t>
+  </si>
+  <si>
+    <t>Ajout de la méthode POST et GET dans le formulaire de création d'annonces + réunion avec le prof concernant le sprint 2 et 3 + supprimer méthode création tableau javascript</t>
+  </si>
+  <si>
+    <t>Documentation faire étape 1 analyse</t>
+  </si>
+  <si>
+    <t>10h35</t>
+  </si>
+  <si>
+    <t>155min</t>
+  </si>
+  <si>
+    <t>Régler problèmes visuels (html css) + documentation</t>
+  </si>
+  <si>
+    <t>35min</t>
   </si>
 </sst>
 </file>
@@ -245,7 +266,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -314,6 +335,7 @@
     <xf numFmtId="11" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="22" fontId="3" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -875,16 +897,16 @@
   <dimension ref="A1:G29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B2" workbookViewId="0">
-      <selection activeCell="G18" sqref="G15:G18"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.7109375" customWidth="1"/>
-    <col min="2" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="22" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="53.5703125" style="27" customWidth="1"/>
   </cols>
@@ -1059,41 +1081,79 @@
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B12" s="11"/>
-      <c r="C12" s="12"/>
-      <c r="D12" s="12"/>
-      <c r="E12" s="13"/>
+    <row r="12" spans="1:7" ht="57.75" x14ac:dyDescent="0.25">
+      <c r="B12" s="11">
+        <v>44244</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="E12" s="30" t="s">
+        <v>22</v>
+      </c>
       <c r="F12" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="G12" s="15"/>
+      <c r="G12" s="15" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B13" s="20"/>
-      <c r="C13" s="16"/>
-      <c r="D13" s="16"/>
-      <c r="E13" s="17"/>
+      <c r="B13" s="20">
+        <v>44246</v>
+      </c>
+      <c r="C13" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="E13" s="17" t="s">
+        <v>22</v>
+      </c>
       <c r="F13" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="G13" s="19"/>
+      <c r="G13" s="19" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B14" s="11"/>
-      <c r="C14" s="16"/>
-      <c r="D14" s="16"/>
-      <c r="E14" s="13"/>
+      <c r="B14" s="11">
+        <v>44256</v>
+      </c>
+      <c r="C14" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="D14" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="E14" s="13" t="s">
+        <v>32</v>
+      </c>
       <c r="F14" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="G14" s="15"/>
+      <c r="G14" s="15" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B15" s="20"/>
-      <c r="C15" s="16"/>
-      <c r="D15" s="16"/>
-      <c r="E15" s="17"/>
+      <c r="B15" s="20">
+        <v>44258</v>
+      </c>
+      <c r="C15" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="D15" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="E15" s="17" t="s">
+        <v>34</v>
+      </c>
       <c r="F15" s="26" t="s">
         <v>9</v>
       </c>

</xml_diff>